<commit_message>
fix: file generator with gender
</commit_message>
<xml_diff>
--- a/assets/source.xlsx
+++ b/assets/source.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2736" yWindow="0" windowWidth="20892" windowHeight="20796" tabRatio="500"/>
+    <workbookView xWindow="2736" yWindow="0" windowWidth="20892" windowHeight="20796" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="variable" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="78">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="80">
   <si>
     <t>Договор</t>
   </si>
@@ -260,6 +260,12 @@
   </si>
   <si>
     <t>3</t>
+  </si>
+  <si>
+    <t>Пол</t>
+  </si>
+  <si>
+    <t>М</t>
   </si>
 </sst>
 </file>
@@ -270,7 +276,7 @@
     <numFmt numFmtId="164" formatCode="#,##0.00&quot; ₽&quot;"/>
     <numFmt numFmtId="165" formatCode="dd\.mm\.yyyy"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="7">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -312,6 +318,13 @@
       <color rgb="FF000000"/>
       <name val="Docs-Times"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
     </font>
   </fonts>
   <fills count="3">
@@ -392,7 +405,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -435,8 +448,13 @@
     <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -821,7 +839,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y1000"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
   <cols>
@@ -2179,8 +2197,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AH1000"/>
   <sheetViews>
-    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="N1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q4" sqref="Q4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4"/>
@@ -2248,7 +2266,9 @@
       <c r="P1" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="Q1" s="3"/>
+      <c r="Q1" s="6" t="s">
+        <v>78</v>
+      </c>
       <c r="R1" s="5"/>
       <c r="S1" s="5"/>
       <c r="T1" s="5"/>
@@ -2316,7 +2336,9 @@
       <c r="P2" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="Q2" s="6"/>
+      <c r="Q2" s="18" t="s">
+        <v>79</v>
+      </c>
       <c r="R2" s="5"/>
       <c r="S2" s="5"/>
       <c r="T2" s="5"/>
@@ -2384,7 +2406,9 @@
       <c r="P3" s="14" t="s">
         <v>46</v>
       </c>
-      <c r="Q3" s="16"/>
+      <c r="Q3" s="17" t="s">
+        <v>79</v>
+      </c>
       <c r="R3" s="5"/>
       <c r="S3" s="5"/>
       <c r="T3" s="5"/>
@@ -2452,7 +2476,9 @@
       <c r="P4" s="14" t="s">
         <v>56</v>
       </c>
-      <c r="Q4" s="16"/>
+      <c r="Q4" s="17" t="s">
+        <v>79</v>
+      </c>
       <c r="R4" s="5"/>
       <c r="S4" s="5"/>
       <c r="T4" s="5"/>
@@ -2520,7 +2546,9 @@
       <c r="P5" s="14" t="s">
         <v>66</v>
       </c>
-      <c r="Q5" s="16"/>
+      <c r="Q5" s="17" t="s">
+        <v>79</v>
+      </c>
       <c r="R5" s="5"/>
       <c r="S5" s="5"/>
       <c r="T5" s="5"/>
@@ -2553,10 +2581,10 @@
       <c r="K6" s="6"/>
       <c r="L6" s="6"/>
       <c r="M6" s="6"/>
-      <c r="N6" s="17"/>
-      <c r="O6" s="17"/>
-      <c r="P6" s="17"/>
-      <c r="Q6" s="17"/>
+      <c r="N6" s="16"/>
+      <c r="O6" s="16"/>
+      <c r="P6" s="16"/>
+      <c r="Q6" s="16"/>
       <c r="R6" s="5"/>
       <c r="S6" s="5"/>
       <c r="T6" s="5"/>
@@ -3701,7 +3729,7 @@
     <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.51180555555555496" footer="0"/>
-  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
   <headerFooter>
     <oddFooter>&amp;C000000&amp;P</oddFooter>
   </headerFooter>

</xml_diff>